<commit_message>
cleaned up git repo, prepare for push
</commit_message>
<xml_diff>
--- a/results_tests/6x_report00.xlsx
+++ b/results_tests/6x_report00.xlsx
@@ -446,127 +446,85 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Kohler</t>
+          <t>Matumona</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alina</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
+          <t>Noe</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kohler</t>
+          <t>Zillig</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nina</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>5.64</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5.75</v>
+          <t>Nicolas</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Matumona</t>
+          <t>Sarman</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Noe</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
+          <t>Dominik</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Matumona</t>
+          <t>Kohler</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nina</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6</v>
+          <t>Alina</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sarman</t>
+          <t>Matumona</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dominik</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4.04</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
+          <t>Nina</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Zillig</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Nicolas</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>4.57</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4.5</v>
+          <t>Marlene</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>Kohler</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Marlene</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>6</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
+          <t>Nina</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented loading classlist from csv and exams from pruefungen.xlsx. Need to test the latter, though
</commit_message>
<xml_diff>
--- a/results_tests/6x_report00.xlsx
+++ b/results_tests/6x_report00.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
debugged loading exams from mem. ready to move on to frontend
</commit_message>
<xml_diff>
--- a/results_tests/6x_report00.xlsx
+++ b/results_tests/6x_report00.xlsx
@@ -446,85 +446,127 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Matumona</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Noe</t>
-        </is>
+          <t>marlene</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5.175109999999999</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Zillig</t>
+          <t>kohler</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nicolas</t>
-        </is>
+          <t>alina</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sarman</t>
+          <t>kohler</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dominik</t>
-        </is>
+          <t>nina</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5.37826</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kohler</t>
+          <t>matumona</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Alina</t>
-        </is>
+          <t>noe</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Matumona</t>
+          <t>matumona</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nina</t>
-        </is>
+          <t>nina</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5.82464</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5.75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>sarman</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Marlene</t>
-        </is>
+          <t>dominik</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4.78031</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4.75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kohler</t>
+          <t>zillig</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nina</t>
-        </is>
+          <t>nicolas</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3.94643</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
found some reasonable GUI package, some progress on how to do stuff wiht it
</commit_message>
<xml_diff>
--- a/results_tests/6x_report00.xlsx
+++ b/results_tests/6x_report00.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>